<commit_message>
Code changes to fix P1 issues
</commit_message>
<xml_diff>
--- a/ICALWS/templates/CorporateActions.xlsx
+++ b/ICALWS/templates/CorporateActions.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ICAL2\temp\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjain\Documents\GitHub\ICAL2.0\ICALWS\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FAD6005A-1BB7-4D43-81DD-E213485C01BE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4F03BFBD-D1CA-4664-945C-96F2F20FD75E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,42 +20,6 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>hchandan</author>
-  </authors>
-  <commentList>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>hchandan:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-date format 
-dd-mm-yyyy
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="205">
   <si>
@@ -678,7 +642,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -812,19 +776,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1168,9 +1119,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -1526,11 +1476,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I1048576"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1541,8 +1491,7 @@
     <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -1574,12 +1523,11 @@
         <v>204</v>
       </c>
     </row>
-    <row r="1048576" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H1048576" s="1"/>
-    </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576" xr:uid="{0A16A0D4-5755-4A13-AACE-D387F27F9893}"/>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -1606,7 +1554,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>197</v>
       </c>
     </row>

</xml_diff>